<commit_message>
working with xl file
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -8,24 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khale\Documents\PYTHON\popularpackages\python-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C75A2-5B58-40B4-BEB9-843F092F0675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B327FE-5BE4-4501-B284-2E613197C084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="3645" windowWidth="24360" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>product_id</t>
   </si>
@@ -34,19 +30,107 @@
   </si>
   <si>
     <t>order_id</t>
+  </si>
+  <si>
+    <t>sales_id</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>Item_id</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>total_amount</t>
+  </si>
+  <si>
+    <t>day_key</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>krishna tolange</t>
+  </si>
+  <si>
+    <t>regular sale</t>
+  </si>
+  <si>
+    <t>dipesh waltson</t>
+  </si>
+  <si>
+    <t>gynandra pandey</t>
+  </si>
+  <si>
+    <t>Pepe Sylvia </t>
+  </si>
+  <si>
+    <t>david clark</t>
+  </si>
+  <si>
+    <t>ram bahadur</t>
+  </si>
+  <si>
+    <t>krishna chanda</t>
+  </si>
+  <si>
+    <t>katrina paudel</t>
+  </si>
+  <si>
+    <t>gorden shumway</t>
+  </si>
+  <si>
+    <t>pratit kunwar</t>
+  </si>
+  <si>
+    <t>puja shakya</t>
+  </si>
+  <si>
+    <t>rita stapit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00;[Red]\-[$$-C09]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -67,15 +151,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{679BA443-43AD-4BB6-BB09-C42BA3212EFD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,7 +480,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -450,4 +540,404 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F82B8A-8D06-4D87-98AA-0F6B3D229CC6}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2019111601</v>
+      </c>
+      <c r="B2" s="2">
+        <v>220160238</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4201911100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>90</v>
+      </c>
+      <c r="G2" s="2">
+        <v>900</v>
+      </c>
+      <c r="H2" s="3">
+        <v>43785</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2019111604</v>
+      </c>
+      <c r="B3" s="2">
+        <v>220120433</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4202009506</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>400</v>
+      </c>
+      <c r="G3" s="2">
+        <v>800</v>
+      </c>
+      <c r="H3" s="3">
+        <v>43788</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2019111605</v>
+      </c>
+      <c r="B4" s="2">
+        <v>220140238</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4202042308</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2">
+        <v>165</v>
+      </c>
+      <c r="H4" s="3">
+        <v>43789</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2019111606</v>
+      </c>
+      <c r="B5" s="2">
+        <v>220091299</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4202075110</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>65</v>
+      </c>
+      <c r="G5" s="2">
+        <v>260</v>
+      </c>
+      <c r="H5" s="3">
+        <v>43790</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2019111607</v>
+      </c>
+      <c r="B6" s="2">
+        <v>220190966</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4202107912</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2">
+        <v>215</v>
+      </c>
+      <c r="H6" s="3">
+        <v>43791</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2019111608</v>
+      </c>
+      <c r="B7" s="2">
+        <v>220140238</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4202140714</v>
+      </c>
+      <c r="E7" s="2">
+        <v>75</v>
+      </c>
+      <c r="F7" s="2">
+        <v>98</v>
+      </c>
+      <c r="G7" s="2">
+        <v>7350</v>
+      </c>
+      <c r="H7" s="3">
+        <v>43792</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2019111609</v>
+      </c>
+      <c r="B8" s="2">
+        <v>220140297</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4202173516</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>432</v>
+      </c>
+      <c r="G8" s="2">
+        <v>864</v>
+      </c>
+      <c r="H8" s="3">
+        <v>43793</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2019111610</v>
+      </c>
+      <c r="B9" s="2">
+        <v>220160238</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4202206318</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>345</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1725</v>
+      </c>
+      <c r="H9" s="3">
+        <v>43794</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2019111611</v>
+      </c>
+      <c r="B10" s="2">
+        <v>220130236</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4202239120</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2">
+        <v>69</v>
+      </c>
+      <c r="H10" s="3">
+        <v>43795</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2019111612</v>
+      </c>
+      <c r="B11" s="2">
+        <v>220130288</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4202271922</v>
+      </c>
+      <c r="E11" s="2">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2">
+        <v>231</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2541</v>
+      </c>
+      <c r="H11" s="3">
+        <v>43796</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2019111613</v>
+      </c>
+      <c r="B12" s="2">
+        <v>220111238</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4202304724</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>680</v>
+      </c>
+      <c r="G12" s="2">
+        <v>680</v>
+      </c>
+      <c r="H12" s="3">
+        <v>43797</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2019111614</v>
+      </c>
+      <c r="B13" s="2">
+        <v>220141132</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4202337526</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2">
+        <v>790</v>
+      </c>
+      <c r="G13" s="2">
+        <v>6320</v>
+      </c>
+      <c r="H13" s="3">
+        <v>43798</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>